<commit_message>
Use digitalOceanService to get database url
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/components.xlsx
+++ b/api/src/DataFixtures/resources/components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85be444a571b20d4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\DataFixtures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CEC8C9E-182E-45C0-955E-75A0F9848766}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6454D801-5E64-4AB3-A592-D7ECFCD7A219}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
   <sheets>
     <sheet name="clusters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>conduction.nl</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>The staging environment</t>
+  </si>
+  <si>
+    <t>conduction</t>
+  </si>
+  <si>
+    <t>zaakonline</t>
   </si>
 </sst>
 </file>
@@ -525,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D686253-1BB3-4847-8D4A-74F469441A53}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +544,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -552,7 +558,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
@@ -721,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6E6857-E780-4091-B7AF-DC1A6A799A18}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix up onto github triggers
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/components.xlsx
+++ b/api/src/DataFixtures/resources/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\DataFixtures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E08AEF-8171-45EF-B5D5-515CB70ACBC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E127538D-514E-4501-866A-793F494DF055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
+    <workbookView xWindow="2730" yWindow="765" windowWidth="21600" windowHeight="15435" activeTab="1" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
   <sheets>
     <sheet name="clusters" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>This common ground component describes common ground components</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/environment-component/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/environment-component/api/helm</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>User Component</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/user-component/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/user-component/api/helm/</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>cgrc</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/Commongroundregistratiecomponent/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/Commongroundregistratiecomponent/api/helm</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>Procesregsitatie Component</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/procesregistratiecomponent/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/procesregistratiecomponent/api/helm</t>
   </si>
   <si>
@@ -100,9 +88,6 @@
     <t>Medewerkercomponent</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/medewerkercatalogus/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/medewerkercatalogus/api/helm</t>
   </si>
   <si>
@@ -112,9 +97,6 @@
     <t>Webresource Catalogus</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/webresourcecatalogus/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/webresourcecatalogus/api/helm</t>
   </si>
   <si>
@@ -124,9 +106,6 @@
     <t>Digispoof UI</t>
   </si>
   <si>
-    <t>https://github.com/ConductionNL/digispoof-interface/</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/digispoof-interface/api/helm</t>
   </si>
   <si>
@@ -167,6 +146,27 @@
   </si>
   <si>
     <t>zaakonline</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/environment-component</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/user-component</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/Commongroundregistratiecomponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/procesregistratiecomponent</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/medewerkercatalogus</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/webresourcecatalogus</t>
+  </si>
+  <si>
+    <t>https://github.com/ConductionNL/digispoof-interface</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D686253-1BB3-4847-8D4A-74F469441A53}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
@@ -544,13 +544,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -558,16 +558,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233B350-72AF-4D84-A15D-5E384E813B54}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,11 +601,11 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -613,16 +613,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -630,16 +630,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -647,16 +647,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -664,16 +664,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -681,16 +681,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -698,16 +698,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -717,9 +717,15 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{CC6D62E1-C4E8-402A-9434-4950A9DB4C39}"/>
     <hyperlink ref="D7" r:id="rId2" xr:uid="{19D77A23-42EE-4254-8245-A81D77BFF7C7}"/>
+    <hyperlink ref="D1" r:id="rId3" xr:uid="{6DB4D0C8-8136-4767-8BB6-9EAFDDDC6960}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{C40D44EA-D742-448C-9AEC-1F4732849AC9}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{50FAC292-CEC4-461E-A9FB-A86D4B7620D5}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{A3D471E1-FC1E-4236-92DC-AC8563A09C8D}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{3FD9B41C-CA07-4E4B-ADC0-B0179A8307EE}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{F7E95135-2938-42E0-8AF7-CA6E5A4EFEF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -740,44 +746,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes up until clusterrolebinding
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/components.xlsx
+++ b/api/src/DataFixtures/resources/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\DataFixtures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E127538D-514E-4501-866A-793F494DF055}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E675474-41EA-4623-9241-9A19E15DA206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="765" windowWidth="21600" windowHeight="15435" activeTab="1" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
   <sheets>
     <sheet name="clusters" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
-  <si>
-    <t>conduction.nl</t>
-  </si>
-  <si>
-    <t>The core conduction cluster</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>evc</t>
   </si>
@@ -109,18 +103,6 @@
     <t>https://github.com/ConductionNL/digispoof-interface/api/helm</t>
   </si>
   <si>
-    <t>zaakonline.nl</t>
-  </si>
-  <si>
-    <t>Het zaakonline cluster</t>
-  </si>
-  <si>
-    <t>The core conduction domain</t>
-  </si>
-  <si>
-    <t>Het zaakonline domain</t>
-  </si>
-  <si>
     <t>dev</t>
   </si>
   <si>
@@ -142,12 +124,6 @@
     <t>The staging environment</t>
   </si>
   <si>
-    <t>conduction</t>
-  </si>
-  <si>
-    <t>zaakonline</t>
-  </si>
-  <si>
     <t>https://github.com/ConductionNL/environment-component</t>
   </si>
   <si>
@@ -167,6 +143,18 @@
   </si>
   <si>
     <t>https://github.com/ConductionNL/digispoof-interface</t>
+  </si>
+  <si>
+    <t>testcluster</t>
+  </si>
+  <si>
+    <t>Een testcluster</t>
+  </si>
+  <si>
+    <t>Een domein voor het testcluster</t>
+  </si>
+  <si>
+    <t>a.conduction.nl</t>
   </si>
 </sst>
 </file>
@@ -529,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D686253-1BB3-4847-8D4A-74F469441A53}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A3:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,30 +532,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -579,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0233B350-72AF-4D84-A15D-5E384E813B54}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,19 +567,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -613,16 +587,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -630,16 +604,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -647,16 +621,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -664,16 +638,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -681,16 +655,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -698,16 +672,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -746,44 +720,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes until github call
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/components.xlsx
+++ b/api/src/DataFixtures/resources/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\environment-component\api\src\DataFixtures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E675474-41EA-4623-9241-9A19E15DA206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E22FBC3-AC9B-4DC1-A3F9-E095D00BE2DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
+    <workbookView xWindow="3510" yWindow="765" windowWidth="21600" windowHeight="15435" xr2:uid="{3860586B-830A-4C68-9AFB-0DF1C2B95B99}"/>
   </bookViews>
   <sheets>
     <sheet name="clusters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>evc</t>
   </si>
@@ -155,6 +155,30 @@
   </si>
   <si>
     <t>a.conduction.nl</t>
+  </si>
+  <si>
+    <t>conduction</t>
+  </si>
+  <si>
+    <t>the main conduction cluster</t>
+  </si>
+  <si>
+    <t>the main conduction domain</t>
+  </si>
+  <si>
+    <t>conduction.nl</t>
+  </si>
+  <si>
+    <t>zaakonline</t>
+  </si>
+  <si>
+    <t>the main zaakonline cluster</t>
+  </si>
+  <si>
+    <t>the main zaakonline domain</t>
+  </si>
+  <si>
+    <t>zaakonline.nl</t>
   </si>
 </sst>
 </file>
@@ -517,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D686253-1BB3-4847-8D4A-74F469441A53}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,15 +556,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>